<commit_message>
atualizei a tabela de dados
</commit_message>
<xml_diff>
--- a/item_4.3_tabela.xlsx
+++ b/item_4.3_tabela.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="178">
   <si>
     <t>-</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Kinoplex Pets</t>
   </si>
   <si>
-    <t>Barra da Tijuca</t>
-  </si>
-  <si>
     <t>Seu Madruga</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Casa Alvorada</t>
   </si>
   <si>
-    <t>Alvorada</t>
-  </si>
-  <si>
     <t>Netuno</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>Pet Feliz</t>
   </si>
   <si>
-    <t>America</t>
-  </si>
-  <si>
     <t>Laranjeiras</t>
   </si>
   <si>
@@ -231,9 +222,6 @@
     <t>Casa do Juju</t>
   </si>
   <si>
-    <t>Ibatiba</t>
-  </si>
-  <si>
     <t>Hebreus lapide</t>
   </si>
   <si>
@@ -297,9 +285,6 @@
     <t>AbraCadabra</t>
   </si>
   <si>
-    <t>Sé Bela Vista</t>
-  </si>
-  <si>
     <t>Galvão Bueno</t>
   </si>
   <si>
@@ -327,9 +312,6 @@
     <t>PronDog</t>
   </si>
   <si>
-    <t>Bento Ferreira</t>
-  </si>
-  <si>
     <t>Amenófis de Assis</t>
   </si>
   <si>
@@ -489,9 +471,6 @@
     <t>cpf_usuario</t>
   </si>
   <si>
-    <t>bairro_usuario</t>
-  </si>
-  <si>
     <t>numero_usuario</t>
   </si>
   <si>
@@ -519,9 +498,6 @@
     <t>nome_casa</t>
   </si>
   <si>
-    <t>bairro_casa</t>
-  </si>
-  <si>
     <t>numero_casa</t>
   </si>
   <si>
@@ -562,6 +538,18 @@
   </si>
   <si>
     <t>nome_estado</t>
+  </si>
+  <si>
+    <t>id_bairro_usuario</t>
+  </si>
+  <si>
+    <t>id_bairro_casa</t>
+  </si>
+  <si>
+    <t>id_bairro</t>
+  </si>
+  <si>
+    <t>nome_bairro</t>
   </si>
 </sst>
 </file>
@@ -955,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI11"/>
+  <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AG17" sqref="AG17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,11 +957,11 @@
     <col min="4" max="4" width="13.44140625" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="28.77734375" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="28.77734375" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
     <col min="12" max="12" width="15.88671875" customWidth="1"/>
     <col min="13" max="13" width="23.5546875" customWidth="1"/>
     <col min="14" max="14" width="18.44140625" customWidth="1"/>
@@ -982,8 +970,7 @@
     <col min="17" max="17" width="14.88671875" customWidth="1"/>
     <col min="18" max="18" width="28.44140625" customWidth="1"/>
     <col min="19" max="19" width="19.77734375" customWidth="1"/>
-    <col min="20" max="20" width="19.6640625" customWidth="1"/>
-    <col min="21" max="21" width="18.44140625" customWidth="1"/>
+    <col min="20" max="21" width="19.6640625" customWidth="1"/>
     <col min="22" max="22" width="16.6640625" customWidth="1"/>
     <col min="23" max="23" width="21.77734375" customWidth="1"/>
     <col min="24" max="24" width="16.88671875" customWidth="1"/>
@@ -993,121 +980,127 @@
     <col min="28" max="28" width="12.44140625" customWidth="1"/>
     <col min="29" max="29" width="17.109375" customWidth="1"/>
     <col min="30" max="30" width="15.44140625" customWidth="1"/>
-    <col min="31" max="31" width="16.88671875" customWidth="1"/>
-    <col min="32" max="32" width="13.5546875" customWidth="1"/>
-    <col min="33" max="33" width="16" customWidth="1"/>
-    <col min="34" max="34" width="14" customWidth="1"/>
-    <col min="35" max="35" width="14.88671875" customWidth="1"/>
+    <col min="31" max="33" width="16.88671875" customWidth="1"/>
+    <col min="34" max="34" width="13.5546875" customWidth="1"/>
+    <col min="35" max="35" width="16" customWidth="1"/>
+    <col min="36" max="36" width="14" customWidth="1"/>
+    <col min="37" max="37" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>181</v>
-      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>8</v>
       </c>
@@ -1127,19 +1120,19 @@
         <v>4</v>
       </c>
       <c r="G2" s="2">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2">
         <v>28990298</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>99999</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="L2" s="2">
         <v>831</v>
@@ -1168,14 +1161,14 @@
       <c r="T2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>14</v>
+      <c r="U2" s="2">
+        <v>6</v>
       </c>
       <c r="V2" s="2">
         <v>100</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>8</v>
@@ -1184,7 +1177,7 @@
         <v>3</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="AA2" s="4">
         <v>43447</v>
@@ -1193,33 +1186,39 @@
         <v>3</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="AD2" s="2">
         <v>2</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AF2" s="2">
         <v>6</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="AH2" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ2" s="2">
         <v>1</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>116</v>
+      <c r="AK2" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4">
         <v>44190</v>
@@ -1231,22 +1230,22 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2">
+        <v>11989325</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2">
-        <v>11989325</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>66666</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="L3" s="2">
         <v>341</v>
@@ -1255,7 +1254,7 @@
         <v>8</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O3" s="2">
         <v>1</v>
@@ -1267,31 +1266,31 @@
         <v>3</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>25</v>
+      <c r="U3" s="2">
+        <v>7</v>
       </c>
       <c r="V3" s="2">
         <v>121</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y3" s="2">
         <v>5</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="AA3" s="4">
         <v>41904</v>
@@ -1300,33 +1299,39 @@
         <v>4</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="AD3" s="2">
         <v>5</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="AF3" s="2">
         <v>7</v>
       </c>
       <c r="AG3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>7</v>
+      </c>
+      <c r="AI3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="AJ3" s="2">
         <v>2</v>
       </c>
-      <c r="AI3" s="2" t="s">
-        <v>120</v>
+      <c r="AK3" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4">
         <v>44234</v>
@@ -1338,22 +1343,22 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>27998029</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="2">
-        <v>27998029</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>22222</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="L4" s="2">
         <v>191</v>
@@ -1362,7 +1367,7 @@
         <v>8</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O4" s="2">
         <v>1</v>
@@ -1374,22 +1379,22 @@
         <v>1</v>
       </c>
       <c r="R4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>37</v>
+      <c r="U4" s="2">
+        <v>3</v>
       </c>
       <c r="V4" s="2">
         <v>167</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>8</v>
@@ -1398,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="AA4" s="4">
         <v>44102</v>
@@ -1407,33 +1412,39 @@
         <v>2</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="AD4" s="2">
         <v>3</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="AF4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH4" s="2">
         <v>3</v>
       </c>
-      <c r="AG4" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AH4" s="2">
+      <c r="AI4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ4" s="2">
         <v>1</v>
       </c>
-      <c r="AI4" s="2" t="s">
-        <v>116</v>
+      <c r="AK4" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4">
         <v>44235</v>
@@ -1445,31 +1456,31 @@
         <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
         <v>27993426</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="2">
+        <v>38</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="2">
         <v>77777</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="L5" s="2">
         <v>561</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O5" s="2">
         <v>1</v>
@@ -1481,31 +1492,31 @@
         <v>4</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="U5" s="2">
+        <v>5</v>
       </c>
       <c r="V5" s="2">
         <v>301</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y5" s="2">
         <v>3</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="AA5" s="4">
         <v>43447</v>
@@ -1514,33 +1525,39 @@
         <v>3</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="AD5" s="2">
         <v>2</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AF5" s="2">
         <v>5</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="AH5" s="2">
+        <v>5</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ5" s="2">
         <v>1</v>
       </c>
-      <c r="AI5" s="2" t="s">
-        <v>116</v>
+      <c r="AK5" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" s="4">
         <v>44114</v>
@@ -1552,22 +1569,22 @@
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G6" s="2">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2">
         <v>27995328</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="2">
+        <v>49</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="2">
         <v>88888</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="L6" s="2">
         <v>912</v>
@@ -1576,34 +1593,34 @@
         <v>8</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="O6" s="2">
         <v>2</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q6" s="2">
         <v>6</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="U6" s="2">
+        <v>4</v>
       </c>
       <c r="V6" s="2">
         <v>62</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>8</v>
@@ -1612,7 +1629,7 @@
         <v>10</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AA6" s="4">
         <v>42324</v>
@@ -1621,33 +1638,39 @@
         <v>9</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="AD6" s="2">
         <v>8</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="AF6" s="2">
         <v>4</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="AH6" s="2">
+        <v>4</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ6" s="2">
         <v>1</v>
       </c>
-      <c r="AI6" s="2" t="s">
-        <v>116</v>
+      <c r="AK6" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4">
         <v>43558</v>
@@ -1659,58 +1682,58 @@
         <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2">
         <v>27980251</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="2">
+        <v>61</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="2">
         <v>55555</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="L7" s="2">
         <v>293</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="O7" s="2">
         <v>2</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="2">
         <v>10</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="U7" s="2">
+        <v>2</v>
       </c>
       <c r="V7" s="2">
         <v>543</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>8</v>
@@ -1719,7 +1742,7 @@
         <v>9</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="AA7" s="4">
         <v>43249</v>
@@ -1728,33 +1751,39 @@
         <v>8</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="AD7" s="2">
         <v>7</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="AF7" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH7" s="2">
         <v>2</v>
       </c>
-      <c r="AG7" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AH7" s="2">
+      <c r="AI7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ7" s="2">
         <v>1</v>
       </c>
-      <c r="AI7" s="2" t="s">
-        <v>116</v>
+      <c r="AK7" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4">
         <v>44084</v>
@@ -1766,67 +1795,67 @@
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G8" s="2">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2">
         <v>21992430</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="2">
+        <v>71</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="2">
         <v>44444</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="L8" s="2">
         <v>555</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="O8" s="2">
         <v>2</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="2">
         <v>7</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="U8" s="2" t="s">
         <v>77</v>
+      </c>
+      <c r="U8" s="2">
+        <v>9</v>
       </c>
       <c r="V8" s="2">
         <v>347</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y8" s="2">
         <v>4</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="AA8" s="4">
         <v>43989</v>
@@ -1835,33 +1864,39 @@
         <v>11</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="AD8" s="2">
         <v>4</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="AF8" s="2">
         <v>9</v>
       </c>
       <c r="AG8" s="2" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="AH8" s="2">
+        <v>9</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ8" s="2">
         <v>4</v>
       </c>
-      <c r="AI8" s="2" t="s">
-        <v>138</v>
+      <c r="AK8" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C9" s="4">
         <v>43801</v>
@@ -1873,67 +1908,67 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G9" s="2">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2">
         <v>55992142</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="2">
+        <v>81</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="2">
         <v>0</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="L9" s="2">
         <v>980</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="O9" s="2">
         <v>3</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Q9" s="2">
         <v>5</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="U9" s="2">
+        <v>10</v>
       </c>
       <c r="V9" s="2">
         <v>296</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y9" s="2">
         <v>7</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="AA9" s="4">
         <v>43750</v>
@@ -1942,33 +1977,39 @@
         <v>6</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AD9" s="2">
         <v>6</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="AF9" s="2">
         <v>10</v>
       </c>
       <c r="AG9" s="2" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="AH9" s="2">
+        <v>10</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ9" s="2">
         <v>5</v>
       </c>
-      <c r="AI9" s="2" t="s">
-        <v>143</v>
+      <c r="AK9" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C10" s="4">
         <v>44105</v>
@@ -1980,67 +2021,67 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
         <v>27994321</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="I10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J10" s="2">
+        <v>91</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="2">
         <v>11111</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="L10" s="2">
         <v>197</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="O10" s="2">
         <v>3</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Q10" s="2">
         <v>2</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
+      </c>
+      <c r="U10" s="2">
+        <v>1</v>
       </c>
       <c r="V10" s="2">
         <v>342</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y10" s="2">
         <v>4</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="AA10" s="4">
         <v>43989</v>
@@ -2049,33 +2090,39 @@
         <v>11</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="AD10" s="2">
         <v>4</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="AF10" s="2">
         <v>1</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="AH10" s="2">
         <v>1</v>
       </c>
       <c r="AI10" s="2" t="s">
-        <v>116</v>
+        <v>138</v>
+      </c>
+      <c r="AJ10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="4">
         <v>42782</v>
@@ -2090,19 +2137,19 @@
         <v>1</v>
       </c>
       <c r="G11" s="2">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2">
         <v>31992435</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J11" s="2">
+        <v>99</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K11" s="2">
         <v>33333</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="L11" s="2">
         <v>455</v>
@@ -2111,43 +2158,43 @@
         <v>8</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="O11" s="2">
         <v>3</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Q11" s="2">
         <v>9</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>87</v>
+        <v>104</v>
+      </c>
+      <c r="U11" s="2">
+        <v>8</v>
       </c>
       <c r="V11" s="2">
         <v>766</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y11" s="2">
         <v>10</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AA11" s="4">
         <v>42324</v>
@@ -2156,25 +2203,31 @@
         <v>9</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="AD11" s="2">
         <v>8</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="AF11" s="2">
         <v>8</v>
       </c>
       <c r="AG11" s="2" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="AH11" s="2">
+        <v>8</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AJ11" s="2">
         <v>3</v>
       </c>
-      <c r="AI11" s="2" t="s">
-        <v>146</v>
+      <c r="AK11" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>